<commit_message>
Double counting: Corrected approach C.
</commit_message>
<xml_diff>
--- a/mappings/mapping.xlsx
+++ b/mappings/mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davidba\internalization\mappings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78459B19-740E-4048-9F9F-615F2495EC50}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9AE5390-FAA1-42A0-89D9-F12AD246C25D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13425" xr2:uid="{6C1C45B8-A416-4819-A2DA-7435EE6C4A6F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13428" activeTab="4" xr2:uid="{6C1C45B8-A416-4819-A2DA-7435EE6C4A6F}"/>
   </bookViews>
   <sheets>
     <sheet name="pe2se" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="190">
   <si>
     <t/>
   </si>
@@ -225,9 +225,6 @@
     <t>electricity production, wind, 1-3MW turbine, offshore</t>
   </si>
   <si>
-    <t>electricity production, wind, 1-3MW turbine, onshore; electricity production, wind, &lt;1MW turbine, onshore; electricity production, wind, &gt;3MW turbine, onshore</t>
-  </si>
-  <si>
     <t>electricity production, deep geothermal</t>
   </si>
   <si>
@@ -240,9 +237,6 @@
     <t>Biodiesel production, via transesterification, from palm oil, energy allocation; Biodiesel production, via transesterification, from rapeseed oil, energy allocation</t>
   </si>
   <si>
-    <t>Ethanol production, via fermentation, from corn, energy allocation</t>
-  </si>
-  <si>
     <t>pegas.seel.ngcc</t>
   </si>
   <si>
@@ -438,9 +432,6 @@
     <t>entyPe</t>
   </si>
   <si>
-    <t>ecoinvent</t>
-  </si>
-  <si>
     <t>crude oil, at production; crude oil, at production offshore</t>
   </si>
   <si>
@@ -507,9 +498,6 @@
     <t>Product shares tbd</t>
   </si>
   <si>
-    <t>petroleum refinery operation</t>
-  </si>
-  <si>
     <t>heat and power co-generation, diesel, 200kW electrical, SCR-NOx reduction</t>
   </si>
   <si>
@@ -540,9 +528,6 @@
     <t>Many ecoinvent options - potentially integrate MAgPIE data?</t>
   </si>
   <si>
-    <t>heat production, hardwood chips from forest, at furnace 1000kW, state-of-the-art 2014</t>
-  </si>
-  <si>
     <t>heat production, natural gas, at industrial furnace &gt;100kW</t>
   </si>
   <si>
@@ -552,12 +537,6 @@
     <t>Already in pe extraction</t>
   </si>
   <si>
-    <t>electricity production, photovoltaic, 570kWp open ground installation, multi-Si</t>
-  </si>
-  <si>
-    <t>electricity production, hydro, run-of-river; electricity production, hydro, pumped storage</t>
-  </si>
-  <si>
     <t>Kerosene production, synthetic, Fischer Tropsch process, hydrogen from wood gasification, with CCS, energy allocation; Diesel production, synthetic, Fischer Tropsch process, hydrogen from wood gasification, with CCS, energy allocation; Naphtha production, synthetic, Fischer Tropsch process, hydrogen from wood gasification, with CCS, energy allocation</t>
   </si>
   <si>
@@ -577,6 +556,60 @@
   </si>
   <si>
     <t>heat and power co-generation, wood chips, 6667 kW</t>
+  </si>
+  <si>
+    <t>heat and power co-generation, hard coal; heat and power co-generation, lignite</t>
+  </si>
+  <si>
+    <t>heat and power co-generation, natural gas, conventional power plant, 100MW electrical</t>
+  </si>
+  <si>
+    <t>mask name</t>
+  </si>
+  <si>
+    <t>mask reference product</t>
+  </si>
+  <si>
+    <t>diesel production, petroleum refinery operation; petrol production, petroleum refinery operation; kerosene production, petroleum refinery operation; heavy fuel oil production, petroleum refinery operation; naphtha production, petroleum refinery operation</t>
+  </si>
+  <si>
+    <t>Not in ecoinvent - Used heat producing process from co-generation</t>
+  </si>
+  <si>
+    <t>electricity</t>
+  </si>
+  <si>
+    <t>Ethanol production, via fermentation</t>
+  </si>
+  <si>
+    <t>economic allocation; system expansion; corn; sorghum; sugarbeet; sugarcane; wheat grains</t>
+  </si>
+  <si>
+    <t>economic allocation; system expansion; wheat straw; eucalyptus; forest residues; miscanthus; poplar; switchgrass; willow</t>
+  </si>
+  <si>
+    <t>electricity production, wind</t>
+  </si>
+  <si>
+    <t>electricity production, hydro</t>
+  </si>
+  <si>
+    <t>electricity production, photovoltaic, commercial</t>
+  </si>
+  <si>
+    <t>offshore; label-certified</t>
+  </si>
+  <si>
+    <t>label-certified</t>
+  </si>
+  <si>
+    <t>heat production, hardwood chips from forest, at furnace 1000kW</t>
+  </si>
+  <si>
+    <t>state-of-the-art</t>
+  </si>
+  <si>
+    <t>hardwood forestry; softwood forestry</t>
   </si>
 </sst>
 </file>
@@ -619,7 +652,13 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="7">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -650,13 +689,15 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="1" xr16:uid="{7B7856A6-CD4E-45B9-8CA8-8CE7C4435C15}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="8" unboundColumnsRight="1">
-    <queryTableFields count="5">
+  <queryTableRefresh nextId="10" unboundColumnsRight="3">
+    <queryTableFields count="7">
       <queryTableField id="2" name="Column2" tableColumnId="2"/>
       <queryTableField id="3" name="Column3" tableColumnId="3"/>
       <queryTableField id="4" name="Column4" tableColumnId="4"/>
       <queryTableField id="6" name="Column6" tableColumnId="6"/>
       <queryTableField id="7" dataBound="0" tableColumnId="5"/>
+      <queryTableField id="8" dataBound="0" tableColumnId="1"/>
+      <queryTableField id="9" dataBound="0" tableColumnId="7"/>
     </queryTableFields>
     <queryTableDeletedFields count="2">
       <deletedField name="Column5"/>
@@ -667,25 +708,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71AD799B-C625-4C9D-8826-5EE8961D9C35}" name="techs" displayName="techs" ref="A1:E49" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:E49" xr:uid="{21954CC5-8FBB-4DFC-987A-0F422035DA4C}"/>
-  <tableColumns count="5">
-    <tableColumn id="2" xr3:uid="{3A879129-1FF8-4009-84A6-F0906898B5D7}" uniqueName="2" name="abbreviation" queryTableFieldId="2" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{2DC3A47D-7F3E-45FC-B487-3208AD4DDB28}" uniqueName="3" name="description" queryTableFieldId="3" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{17F12A7F-754B-4AB5-8046-5024FADDD075}" uniqueName="4" name="is pe2se" queryTableFieldId="4" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{511B1039-CAA1-4A68-BFF6-C5BD390A81B1}" uniqueName="6" name="ecoinvent name" queryTableFieldId="6" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{8428EB48-ED85-4048-8FEA-77F177CD2796}" uniqueName="5" name="note" queryTableFieldId="7" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{71AD799B-C625-4C9D-8826-5EE8961D9C35}" name="techs" displayName="techs" ref="A1:G49" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:G49" xr:uid="{21954CC5-8FBB-4DFC-987A-0F422035DA4C}"/>
+  <tableColumns count="7">
+    <tableColumn id="2" xr3:uid="{3A879129-1FF8-4009-84A6-F0906898B5D7}" uniqueName="2" name="abbreviation" queryTableFieldId="2" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{2DC3A47D-7F3E-45FC-B487-3208AD4DDB28}" uniqueName="3" name="description" queryTableFieldId="3" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{17F12A7F-754B-4AB5-8046-5024FADDD075}" uniqueName="4" name="is pe2se" queryTableFieldId="4" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{511B1039-CAA1-4A68-BFF6-C5BD390A81B1}" uniqueName="6" name="ecoinvent name" queryTableFieldId="6" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{8428EB48-ED85-4048-8FEA-77F177CD2796}" uniqueName="5" name="note" queryTableFieldId="7" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{F1FDF344-7626-40D7-9ACD-4D3F79182323}" uniqueName="1" name="mask name" queryTableFieldId="8" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{3FD9109E-8EA6-42F8-9EA2-1DB10CA4CC6A}" uniqueName="7" name="mask reference product" queryTableFieldId="9" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D236F856-7534-4E09-AEBB-7419DFA18DAC}" name="Table2" displayName="Table2" ref="A1:B12" totalsRowShown="0">
-  <autoFilter ref="A1:B12" xr:uid="{23DD6F09-CFEC-442C-9675-DC47C10E26BA}"/>
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D236F856-7534-4E09-AEBB-7419DFA18DAC}" name="Table2" displayName="Table2" ref="A1:D12" totalsRowShown="0">
+  <autoFilter ref="A1:D12" xr:uid="{23DD6F09-CFEC-442C-9675-DC47C10E26BA}"/>
+  <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{767D8F58-C529-4FE8-B59A-A2855066DDA2}" name="entyPe"/>
-    <tableColumn id="2" xr3:uid="{B8A862D3-3DFE-43FB-8A84-58BD6CA093DC}" name="ecoinvent"/>
+    <tableColumn id="2" xr3:uid="{B8A862D3-3DFE-43FB-8A84-58BD6CA093DC}" name="ecoinvent name"/>
+    <tableColumn id="3" xr3:uid="{0896B9D1-FB48-4B75-849D-C953978C372F}" name="mask name"/>
+    <tableColumn id="4" xr3:uid="{FCD14A82-4AF5-44D5-BABE-A98E2A0EFC51}" name="mask reference product"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -988,21 +1033,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50CA17E1-7C3F-4153-831B-D0822849F9D4}">
-  <dimension ref="A1:E91"/>
+  <dimension ref="A1:G91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" customWidth="1"/>
-    <col min="2" max="2" width="81.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="57.140625" customWidth="1"/>
+    <col min="1" max="1" width="30.33203125" customWidth="1"/>
+    <col min="2" max="2" width="81.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="57.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>52</v>
       </c>
@@ -1016,12 +1061,18 @@
         <v>55</v>
       </c>
       <c r="E1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+      <c r="F1" t="s">
+        <v>174</v>
+      </c>
+      <c r="G1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
@@ -1033,10 +1084,12 @@
         <v>56</v>
       </c>
       <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
@@ -1045,13 +1098,15 @@
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>5</v>
@@ -1063,10 +1118,12 @@
         <v>57</v>
       </c>
       <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
@@ -1076,12 +1133,14 @@
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>7</v>
@@ -1090,15 +1149,17 @@
         <v>2</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>0</v>
+        <v>173</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>8</v>
@@ -1107,15 +1168,17 @@
         <v>2</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>9</v>
@@ -1127,10 +1190,12 @@
         <v>58</v>
       </c>
       <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>10</v>
@@ -1142,10 +1207,12 @@
         <v>59</v>
       </c>
       <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>11</v>
@@ -1157,12 +1224,14 @@
         <v>0</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>12</v>
@@ -1174,12 +1243,14 @@
         <v>0</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>13</v>
@@ -1188,15 +1259,17 @@
         <v>2</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>155</v>
+        <v>176</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>14</v>
@@ -1205,15 +1278,17 @@
         <v>2</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>15</v>
@@ -1222,15 +1297,17 @@
         <v>2</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>16</v>
@@ -1239,15 +1316,17 @@
         <v>2</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>17</v>
@@ -1256,13 +1335,15 @@
         <v>2</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>18</v>
@@ -1271,15 +1352,17 @@
         <v>2</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>0</v>
+        <v>172</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>19</v>
@@ -1288,15 +1371,19 @@
         <v>2</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>0</v>
+        <v>172</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>20</v>
@@ -1305,15 +1392,17 @@
         <v>2</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>21</v>
@@ -1322,15 +1411,17 @@
         <v>2</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>22</v>
@@ -1339,13 +1430,15 @@
         <v>2</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>23</v>
@@ -1354,13 +1447,15 @@
         <v>2</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="E22" s="1"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>24</v>
@@ -1369,13 +1464,15 @@
         <v>2</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>25</v>
@@ -1384,13 +1481,15 @@
         <v>2</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>26</v>
@@ -1399,15 +1498,17 @@
         <v>27</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>28</v>
@@ -1416,15 +1517,17 @@
         <v>27</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>29</v>
@@ -1433,15 +1536,17 @@
         <v>27</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>30</v>
@@ -1450,13 +1555,17 @@
         <v>27</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>166</v>
+        <v>187</v>
       </c>
       <c r="E28" s="1"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>31</v>
@@ -1465,13 +1574,15 @@
         <v>27</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E29" s="1"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>32</v>
@@ -1480,13 +1591,15 @@
         <v>27</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E30" s="1"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>33</v>
@@ -1495,13 +1608,15 @@
         <v>27</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E31" s="1"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>34</v>
@@ -1510,13 +1625,15 @@
         <v>27</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E32" s="1"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>35</v>
@@ -1525,13 +1642,15 @@
         <v>27</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="E33" s="1"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>36</v>
@@ -1540,13 +1659,15 @@
         <v>27</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="E34" s="1"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>37</v>
@@ -1555,13 +1676,15 @@
         <v>27</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E35" s="1"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>38</v>
@@ -1570,13 +1693,15 @@
         <v>27</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E36" s="1"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>39</v>
@@ -1585,15 +1710,19 @@
         <v>27</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>0</v>
+        <v>179</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="G37" s="1"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>40</v>
@@ -1602,15 +1731,19 @@
         <v>27</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>66</v>
+        <v>179</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="G38" s="1"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>41</v>
@@ -1619,13 +1752,15 @@
         <v>27</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E39" s="1"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>42</v>
@@ -1634,13 +1769,15 @@
         <v>27</v>
       </c>
       <c r="D40" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E40" s="1"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>43</v>
@@ -1649,13 +1786,15 @@
         <v>27</v>
       </c>
       <c r="D41" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E41" s="1"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>44</v>
@@ -1664,15 +1803,17 @@
         <v>27</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>171</v>
+        <v>183</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>45</v>
@@ -1681,13 +1822,17 @@
         <v>27</v>
       </c>
       <c r="D43" t="s">
-        <v>61</v>
+        <v>182</v>
       </c>
       <c r="E43" s="1"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F43" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="G43" s="1"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>46</v>
@@ -1699,10 +1844,14 @@
         <v>60</v>
       </c>
       <c r="E44" s="1"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F44" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G44" s="1"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>47</v>
@@ -1711,15 +1860,17 @@
         <v>27</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>170</v>
+        <v>184</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>48</v>
@@ -1728,13 +1879,15 @@
         <v>27</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E46" s="1"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>49</v>
@@ -1744,12 +1897,14 @@
       </c>
       <c r="D47" s="1"/>
       <c r="E47" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>50</v>
@@ -1758,13 +1913,15 @@
         <v>27</v>
       </c>
       <c r="D48" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E48" s="1"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>51</v>
@@ -1773,13 +1930,15 @@
         <v>27</v>
       </c>
       <c r="D49" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1" t="s">
@@ -1790,7 +1949,7 @@
       </c>
       <c r="E50" s="1"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1" t="s">
@@ -1801,7 +1960,7 @@
       </c>
       <c r="E51" s="1"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1" t="s">
@@ -1812,7 +1971,7 @@
       </c>
       <c r="E52" s="1"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1" t="s">
@@ -1823,7 +1982,7 @@
       </c>
       <c r="E53" s="1"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1" t="s">
@@ -1834,7 +1993,7 @@
       </c>
       <c r="E54" s="1"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1" t="s">
@@ -1845,7 +2004,7 @@
       </c>
       <c r="E55" s="1"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1" t="s">
@@ -1856,7 +2015,7 @@
       </c>
       <c r="E56" s="1"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1" t="s">
@@ -1867,7 +2026,7 @@
       </c>
       <c r="E57" s="1"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1" t="s">
@@ -1878,7 +2037,7 @@
       </c>
       <c r="E58" s="1"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1" t="s">
@@ -1889,7 +2048,7 @@
       </c>
       <c r="E59" s="1"/>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1" t="s">
@@ -1900,7 +2059,7 @@
       </c>
       <c r="E60" s="1"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1" t="s">
@@ -1911,7 +2070,7 @@
       </c>
       <c r="E61" s="1"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1" t="s">
@@ -1922,7 +2081,7 @@
       </c>
       <c r="E62" s="1"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1" t="s">
@@ -1933,7 +2092,7 @@
       </c>
       <c r="E63" s="1"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1" t="s">
@@ -1944,7 +2103,7 @@
       </c>
       <c r="E64" s="1"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1" t="s">
@@ -1955,7 +2114,7 @@
       </c>
       <c r="E65" s="1"/>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1" t="s">
@@ -1966,7 +2125,7 @@
       </c>
       <c r="E66" s="1"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1" t="s">
@@ -1977,7 +2136,7 @@
       </c>
       <c r="E67" s="1"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1" t="s">
@@ -1988,7 +2147,7 @@
       </c>
       <c r="E68" s="1"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1" t="s">
@@ -1999,7 +2158,7 @@
       </c>
       <c r="E69" s="1"/>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1" t="s">
@@ -2010,7 +2169,7 @@
       </c>
       <c r="E70" s="1"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1" t="s">
@@ -2021,7 +2180,7 @@
       </c>
       <c r="E71" s="1"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1" t="s">
@@ -2032,7 +2191,7 @@
       </c>
       <c r="E72" s="1"/>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1" t="s">
@@ -2043,7 +2202,7 @@
       </c>
       <c r="E73" s="1"/>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1" t="s">
@@ -2054,7 +2213,7 @@
       </c>
       <c r="E74" s="1"/>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1" t="s">
@@ -2065,7 +2224,7 @@
       </c>
       <c r="E75" s="1"/>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1" t="s">
@@ -2076,7 +2235,7 @@
       </c>
       <c r="E76" s="1"/>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1" t="s">
@@ -2087,7 +2246,7 @@
       </c>
       <c r="E77" s="1"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1" t="s">
@@ -2098,7 +2257,7 @@
       </c>
       <c r="E78" s="1"/>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1" t="s">
@@ -2109,7 +2268,7 @@
       </c>
       <c r="E79" s="1"/>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1" t="s">
@@ -2120,7 +2279,7 @@
       </c>
       <c r="E80" s="1"/>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1" t="s">
@@ -2131,7 +2290,7 @@
       </c>
       <c r="E81" s="1"/>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1" t="s">
@@ -2142,7 +2301,7 @@
       </c>
       <c r="E82" s="1"/>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1" t="s">
@@ -2153,7 +2312,7 @@
       </c>
       <c r="E83" s="1"/>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1" t="s">
@@ -2164,7 +2323,7 @@
       </c>
       <c r="E84" s="1"/>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1" t="s">
@@ -2175,7 +2334,7 @@
       </c>
       <c r="E85" s="1"/>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1" t="s">
@@ -2186,7 +2345,7 @@
       </c>
       <c r="E86" s="1"/>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1" t="s">
@@ -2197,7 +2356,7 @@
       </c>
       <c r="E87" s="1"/>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1" t="s">
@@ -2208,7 +2367,7 @@
       </c>
       <c r="E88" s="1"/>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1" t="s">
@@ -2219,7 +2378,7 @@
       </c>
       <c r="E89" s="1"/>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1" t="s">
@@ -2230,7 +2389,7 @@
       </c>
       <c r="E90" s="1"/>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1" t="s">
@@ -2256,7 +2415,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2268,7 +2427,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2280,7 +2439,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2288,103 +2447,112 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{314D3D07-1E74-4015-9294-D84392A15524}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B3" t="s">
         <v>131</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B4" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>120</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B5" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>121</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>122</v>
+      </c>
+      <c r="B6" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>122</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>123</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B8" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>124</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>125</v>
+      </c>
+      <c r="B9" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>125</v>
-      </c>
-      <c r="B7" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>126</v>
       </c>
-      <c r="B8" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B10" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>127</v>
       </c>
-      <c r="B9" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>128</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>